<commit_message>
adding my newest experiments
</commit_message>
<xml_diff>
--- a/s2cDNASample/s2cDNASample_H.BROWN_08.27.20.xlsx
+++ b/s2cDNASample/s2cDNASample_H.BROWN_08.27.20.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s2cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01990166-FC95-524B-96D5-8C2FCBE6774E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12066CD-BF7D-F94D-A509-3DBF44DC51DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1980" windowWidth="27640" windowHeight="16940" xr2:uid="{342F322B-E5C6-9F45-A0D8-2419A7922C20}"/>
+    <workbookView xWindow="680" yWindow="2400" windowWidth="27640" windowHeight="16940" xr2:uid="{342F322B-E5C6-9F45-A0D8-2419A7922C20}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D9"/>
+      <selection activeCell="A2" sqref="A2:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>